<commit_message>
dynamic changes of site has been found and made changes in the code
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/ChatBot Chat Suggestions.xlsx
+++ b/src/main/resources/testdata/ChatBot Chat Suggestions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\268850\Capstone-workspace\lenskart-qa\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\268850\Capstone-workspace\lenskart-qa\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B0A9AC-FDC5-44D5-94ED-0F861F8D5742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBE1F17-921F-4933-9391-156BC868A903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="2840" windowWidth="14400" windowHeight="7360" xr2:uid="{AC677EEA-AA55-4D60-9803-FFD1085D5371}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AC677EEA-AA55-4D60-9803-FFD1085D5371}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -82,12 +82,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -102,9 +108,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,20 +429,20 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="29.36328125" customWidth="1"/>
-    <col min="2" max="2" width="64.08984375" customWidth="1"/>
+    <col min="2" max="2" width="59.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>